<commit_message>
feat: Atualização do conteúdo de aula dado em 2023 para as turmas de fev e ago.
</commit_message>
<xml_diff>
--- a/00 Plano de Aula/edge_computing_computer_systems_2023.xlsx
+++ b/00 Plano de Aula/edge_computing_computer_systems_2023.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google Drive\Profissional\Empresas\FIAP\02 Aulas\Engenharia de Software\Edge Computing\00 Plano de Aula\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google Drive\Profissional\Empresas\02. FIAP\02 Aulas\1ES\Edge Computing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84202EFB-0B1F-4090-95A3-3739BA976B63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84EDA07F-431F-4EF7-8B74-F2931AB14B64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{D49DE45F-6E56-49B0-AF9E-35E4A8BA3329}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D49DE45F-6E56-49B0-AF9E-35E4A8BA3329}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="43">
   <si>
     <t>DISCIPLINA:</t>
   </si>
@@ -126,23 +126,74 @@
     <t xml:space="preserve">Bootloade, ICSP, Interrupções e Whatchdog </t>
   </si>
   <si>
-    <t>Serial Temperature Sensor, Light Sensor e/ou Ultrassonic Radar</t>
-  </si>
-  <si>
-    <t>Mood Lamp, Fire Effect,  Mood Lamp e/ou Piezo Sounder Melody Player</t>
-  </si>
-  <si>
     <t>Interactive Traffic, Chase Effect, Interactive Chase Effect e/ou Pulsating Lamp</t>
   </si>
   <si>
     <t>Data logger e Gravação EEPROM</t>
+  </si>
+  <si>
+    <t>ESPX</t>
+  </si>
+  <si>
+    <t>ESPW</t>
+  </si>
+  <si>
+    <t>ESPV</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>Check Point 01 - Light Sensor</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Mood Lamp, Fire Effect,  Mood Lamp </t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>e/ou Piezo Sounder Melody Player</t>
+    </r>
+  </si>
+  <si>
+    <t>Check Point 02 - Serial Temperature Sensor (DHT) e Display</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Serial Temperature Sensor, Light Sensor e/ou  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Piezo Sounder Melody Player e Ultrassonic Radar e sensor de presença</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -188,8 +239,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <strike/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -218,6 +277,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -335,7 +400,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -376,6 +441,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -391,6 +459,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -705,25 +774,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61519789-C00C-41BB-A46E-0B2341A8977A}">
-  <dimension ref="A1:B46"/>
+  <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="93.85546875" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="93.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="15"/>
-    </row>
-    <row r="2" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="16"/>
+    </row>
+    <row r="2" spans="1:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -731,7 +800,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -739,187 +808,361 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="16" t="s">
+    <row r="4" spans="1:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="17"/>
-    </row>
-    <row r="5" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="18"/>
+    </row>
+    <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5">
         <v>1</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="7">
         <v>2</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="7">
         <v>3</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="7">
         <v>4</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+      <c r="C9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="7">
         <v>5</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+      <c r="C10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="7">
         <v>6</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+      <c r="C11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="7">
         <v>7</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+      <c r="C12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="7">
         <v>8</v>
       </c>
       <c r="B13" s="13" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
+    </row>
+    <row r="14" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="7">
         <v>9</v>
       </c>
       <c r="B14" s="8" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C14" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" t="s">
+        <v>38</v>
+      </c>
+      <c r="E14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="7">
         <v>10</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+      <c r="C15" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="7">
         <v>11</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+      <c r="C16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" t="s">
+        <v>38</v>
+      </c>
+      <c r="E16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="7">
         <v>12</v>
       </c>
       <c r="B17" s="13" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C17" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" t="s">
+        <v>38</v>
+      </c>
+      <c r="E17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="7">
         <v>13</v>
       </c>
       <c r="B18" s="13" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C18" s="20"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
+    </row>
+    <row r="19" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="7">
         <v>14</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="14" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C19" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" t="s">
+        <v>38</v>
+      </c>
+      <c r="E19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="7">
         <v>15</v>
       </c>
       <c r="B20" s="9" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" t="s">
+        <v>38</v>
+      </c>
+      <c r="E20" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="7">
         <v>16</v>
       </c>
       <c r="B21" s="11" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C21" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21" t="s">
+        <v>38</v>
+      </c>
+      <c r="E21" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="7">
         <v>17</v>
       </c>
       <c r="B22" s="11" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C22" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" t="s">
+        <v>38</v>
+      </c>
+      <c r="E22" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="7">
         <v>18</v>
       </c>
       <c r="B23" s="11" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C23" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" t="s">
+        <v>38</v>
+      </c>
+      <c r="E23" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="7">
         <v>19</v>
       </c>
       <c r="B24" s="11" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C24" t="s">
+        <v>38</v>
+      </c>
+      <c r="D24" t="s">
+        <v>38</v>
+      </c>
+      <c r="E24" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="7">
         <v>20</v>
       </c>
       <c r="B25" s="11" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="16" t="s">
+      <c r="C25" t="s">
+        <v>38</v>
+      </c>
+      <c r="D25" t="s">
+        <v>38</v>
+      </c>
+      <c r="E25" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B26" s="18"/>
-    </row>
-    <row r="27" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="19"/>
+    </row>
+    <row r="27" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="7">
         <v>1</v>
       </c>
@@ -927,7 +1170,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="7">
         <v>2</v>
       </c>
@@ -935,7 +1178,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="7">
         <v>3</v>
       </c>
@@ -943,7 +1186,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="7">
         <v>4</v>
       </c>
@@ -951,7 +1194,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="7">
         <v>5</v>
       </c>
@@ -959,7 +1202,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="7">
         <v>6</v>
       </c>
@@ -967,7 +1210,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="7">
         <v>7</v>
       </c>
@@ -975,7 +1218,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="7">
         <v>8</v>
       </c>
@@ -983,7 +1226,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="7">
         <v>9</v>
       </c>
@@ -991,7 +1234,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="7">
         <v>10</v>
       </c>
@@ -999,7 +1242,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="7">
         <v>11</v>
       </c>
@@ -1007,7 +1250,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="7">
         <v>12</v>
       </c>
@@ -1015,7 +1258,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="7">
         <v>13</v>
       </c>
@@ -1023,7 +1266,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="7">
         <v>14</v>
       </c>
@@ -1031,7 +1274,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="7">
         <v>15</v>
       </c>
@@ -1039,7 +1282,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="7">
         <v>16</v>
       </c>
@@ -1047,7 +1290,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="7">
         <v>17</v>
       </c>
@@ -1055,7 +1298,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="7">
         <v>18</v>
       </c>
@@ -1063,7 +1306,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="7">
         <v>19</v>
       </c>
@@ -1071,7 +1314,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="7">
         <v>20</v>
       </c>
@@ -1086,6 +1329,6 @@
     <mergeCell ref="A26:B26"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>